<commit_message>
Update DateBase/orders/International Ever Green_2024-12-24.xlsx
</commit_message>
<xml_diff>
--- a/DateBase/orders/International Ever Green_2024-12-24.xlsx
+++ b/DateBase/orders/International Ever Green_2024-12-24.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -527,9 +527,92 @@
         <v>8</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>3</v>
+      </c>
+      <c r="C12" t="str">
+        <v>192_粉荔枝_Pink Ohara_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F12" t="str">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" t="str">
+        <v>197_粉红雪山_Sweet Avalanche_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F13" t="str">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" t="str">
+        <v>192_粉荔枝_Pink Ohara_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F14" t="str">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" t="str">
+        <v>148_坦尼克_Tineke_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F15" t="str">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" t="str">
+        <v>479_绿灵草_lepidium_undefined_1bunch</v>
+      </c>
+      <c r="F16" t="str">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>4</v>
+      </c>
+      <c r="C17" t="str">
+        <v>138_卡罗拉_Carola_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F17" t="str">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="C18" t="str">
+        <v>148_坦尼克_Tineke_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F18" t="str">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="C19" t="str">
+        <v>173_朱丽叶_Juliet_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F19" t="str">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" t="str">
+        <v>209_海洋之歌_Ocean Song_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F20" t="str">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" t="str">
+        <v>184_微光_shimmer_Rosa rugosa Thunb._20stems</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L21"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -587,7 +670,7 @@
         <v>0.00</v>
       </c>
       <c r="G2" t="str">
-        <v>0101367310281538</v>
+        <v>01013673102815383151019251841180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>